<commit_message>
Botón cancelar, falta editar cliente
</commit_message>
<xml_diff>
--- a/Requerimientos/Tabla de requerimientos SGP.xlsx
+++ b/Requerimientos/Tabla de requerimientos SGP.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DPAREJA/git/SGP/Requerimientos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpareja/SGP/Requerimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A38AC78-CFBA-8C45-B976-BD1D3D4ED9CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15260" tabRatio="990"/>
+    <workbookView xWindow="3420" yWindow="0" windowWidth="20480" windowHeight="15260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,6 +244,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -509,11 +513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Registrar Historias de Usuario
</commit_message>
<xml_diff>
--- a/Requerimientos/Tabla de requerimientos SGP.xlsx
+++ b/Requerimientos/Tabla de requerimientos SGP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpareja/SGP/Requerimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EE45E3-7704-6345-8F59-B9F62DD17A78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A086BC-4958-8149-9773-32187990A634}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="0" windowWidth="20480" windowHeight="15260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ver historias de usuario, filtrar
</commit_message>
<xml_diff>
--- a/Requerimientos/Tabla de requerimientos SGP.xlsx
+++ b/Requerimientos/Tabla de requerimientos SGP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpareja/SGP/Requerimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A086BC-4958-8149-9773-32187990A634}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F7B651-00DA-CC49-B4FA-73BB71065293}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="0" windowWidth="20480" windowHeight="15260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4560" yWindow="0" windowWidth="20480" windowHeight="15260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Borrar la información del txt de Requisito cuando le de en limpiar, en la pantalla de historias de usuario
</commit_message>
<xml_diff>
--- a/Requerimientos/Tabla de requerimientos SGP.xlsx
+++ b/Requerimientos/Tabla de requerimientos SGP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpareja/SGP/Requerimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F7B651-00DA-CC49-B4FA-73BB71065293}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E786E1-5F54-9A44-9BE7-34B32A35D0BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="0" windowWidth="20480" windowHeight="15260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Poder guardar actividades dentro del proyecto asignando la historia de usuario asoaciada a la actividad
</commit_message>
<xml_diff>
--- a/Requerimientos/Tabla de requerimientos SGP.xlsx
+++ b/Requerimientos/Tabla de requerimientos SGP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpareja/SGP/Requerimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E786E1-5F54-9A44-9BE7-34B32A35D0BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1E6B12-EC4A-F243-A795-B4251B8A850D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="0" windowWidth="20480" windowHeight="15260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -591,7 +591,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -599,7 +599,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>